<commit_message>
15th commit - Data-driven - Adding Data Provider and Create another test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -338,9 +338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
24th commit - Data-driven - Adding Data Provider and Create another test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -24,21 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>postCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Janielle Joy</t>
   </si>
   <si>
     <t>Gregorio</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -365,38 +371,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>1700</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st commit - Data-driven - Creating a common data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Janielle Joy</t>
   </si>
@@ -45,6 +46,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Janielle Joy Gregorio</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -373,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,4 +429,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
6th commit - Data-driven - Adding parameterization
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="810"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Janielle Joy</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Dollar</t>
+  </si>
+  <si>
+    <t>Ed</t>
+  </si>
+  <si>
+    <t>Sheeran</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Kitty</t>
   </si>
 </sst>
 </file>
@@ -384,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,6 +443,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>1800</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>1989</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>8888</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -435,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1st commit - Data-driven - Adding parameterization
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="810"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Janielle Joy</t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t>Kitty</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -402,10 +421,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
2nd commit - Data-driven - Run modes for test suite data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Janielle Joy</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -138,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +431,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +440,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -471,10 +478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +491,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -497,8 +504,11 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -511,8 +521,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -525,8 +538,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -539,8 +555,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -552,6 +571,9 @@
       </c>
       <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issues in hashtable
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -12,9 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="810"/>
   </bookViews>
   <sheets>
-    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Janielle Joy</t>
   </si>
@@ -77,30 +76,6 @@
   </si>
   <si>
     <t>Kitty</t>
-  </si>
-  <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>runmode</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -144,10 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,60 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +415,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,11 +428,8 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -521,11 +442,8 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -538,11 +456,8 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -555,11 +470,8 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -571,9 +483,6 @@
       </c>
       <c r="D5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>